<commit_message>
fixat edit schema och ny schematid
</commit_message>
<xml_diff>
--- a/Excel/Grunddata.xlsx
+++ b/Excel/Grunddata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AlbinÖstholm\Documents\Harohal\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AlbinÖstholm\Documents\harohal\Harohal\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,18 +17,19 @@
     <sheet name="vecka 48" sheetId="12" r:id="rId3"/>
     <sheet name="vecka_49" sheetId="14" r:id="rId4"/>
     <sheet name="vecka_50" sheetId="18" r:id="rId5"/>
-    <sheet name="Blad5" sheetId="16" r:id="rId6"/>
-    <sheet name="ADventofcode" sheetId="13" r:id="rId7"/>
-    <sheet name="Ett fucking blad" sheetId="17" r:id="rId8"/>
-    <sheet name="Ordrar" sheetId="9" r:id="rId9"/>
-    <sheet name="Nyheter" sheetId="8" r:id="rId10"/>
-    <sheet name="Tjanster" sheetId="7" r:id="rId11"/>
-    <sheet name="Anstallda" sheetId="6" r:id="rId12"/>
-    <sheet name="Annonser" sheetId="4" r:id="rId13"/>
-    <sheet name="Personer" sheetId="3" r:id="rId14"/>
-    <sheet name="Artikel" sheetId="5" r:id="rId15"/>
-    <sheet name="Schema" sheetId="2" r:id="rId16"/>
-    <sheet name="Blad1" sheetId="15" r:id="rId17"/>
+    <sheet name="vecka_8" sheetId="19" r:id="rId6"/>
+    <sheet name="Blad5" sheetId="16" r:id="rId7"/>
+    <sheet name="ADventofcode" sheetId="13" r:id="rId8"/>
+    <sheet name="Ett fucking blad" sheetId="17" r:id="rId9"/>
+    <sheet name="Ordrar" sheetId="9" r:id="rId10"/>
+    <sheet name="Nyheter" sheetId="8" r:id="rId11"/>
+    <sheet name="Tjanster" sheetId="7" r:id="rId12"/>
+    <sheet name="Anstallda" sheetId="6" r:id="rId13"/>
+    <sheet name="Annonser" sheetId="4" r:id="rId14"/>
+    <sheet name="Personer" sheetId="3" r:id="rId15"/>
+    <sheet name="Artikel" sheetId="5" r:id="rId16"/>
+    <sheet name="Schema" sheetId="2" r:id="rId17"/>
+    <sheet name="Blad1" sheetId="15" r:id="rId18"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="226">
   <si>
     <t>Namn</t>
   </si>
@@ -676,6 +677,48 @@
   </si>
   <si>
     <t>INSERT INTO ordrar(tjanstID, anstalldID, personID, startTid, slutTid,CreatedBy) VALUES('1','A3B762F3-79F8-49B2-8722-354505C82FF4','095C51B3-C019-49F4-B80F-E4CEEADA3504', '2016-12-16 16:00:00.000', '2016-12-16 17:00:00.000','A3B762F3-79F8-49B2-8722-354505C82FF4')</t>
+  </si>
+  <si>
+    <t>2017-02-21  10:30:00.00</t>
+  </si>
+  <si>
+    <t>2017-02-21  13:00:00.00</t>
+  </si>
+  <si>
+    <t>2017-02-21  14:30:00.00</t>
+  </si>
+  <si>
+    <t>2017-02-21  20:00:00.00</t>
+  </si>
+  <si>
+    <t>2017-02-22  10:00:00.00</t>
+  </si>
+  <si>
+    <t>2017-02-22  14:30:00.00</t>
+  </si>
+  <si>
+    <t>2017-02-22  14:00:00.00</t>
+  </si>
+  <si>
+    <t>2017-02-22  21:00:00.00</t>
+  </si>
+  <si>
+    <t>2017-02-23  12:00:00.00</t>
+  </si>
+  <si>
+    <t>2017-02-23  16:30:00.00</t>
+  </si>
+  <si>
+    <t>2017-02-23  16:00:00.00</t>
+  </si>
+  <si>
+    <t>2017-02-23  20:30:00.00</t>
+  </si>
+  <si>
+    <t>StartTid</t>
+  </si>
+  <si>
+    <t>SlutTid</t>
   </si>
 </sst>
 </file>
@@ -1148,6 +1191,302 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L20"/>
+  <sheetViews>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="22" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="255.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2" s="6">
+        <v>1</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E2" s="6">
+        <v>0</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="I2" s="6">
+        <v>1</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5" t="str">
+        <f>"INSERT INTO ordrar(orderID, tjanstID, anstalldID, personID, betald, orderdatum, starttid, sluttid, aktiv, createdBy) VALUES('"&amp;A2&amp;"','"&amp;B2&amp;"','"&amp;C2&amp;"','"&amp;D2&amp;"','"&amp;E2&amp;"','"&amp;F2&amp;"','"&amp;G2&amp;"','"&amp;H2&amp;"','"&amp;I2&amp;"','"&amp;J2&amp;"')"</f>
+        <v>INSERT INTO ordrar(orderID, tjanstID, anstalldID, personID, betald, orderdatum, starttid, sluttid, aktiv, createdBy) VALUES('0F51A3C3-D37C-444D-9D9A-7DA5C995837C','1','A3B762F3-79F8-49B2-8722-354505C82FF4','9E0C52CD-9F2C-432C-A6C1-D2475B5315D3','0','2016-11-14 08:46:18.427','2016-11-15 08:36:14.330','2016-11-15 10:36:14.330','1','A3B762F3-79F8-49B2-8722-354505C82FF4')</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="L5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="L6" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="L7" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="L8" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="L9" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="L10" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="L11" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="L12" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="L13" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L14" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L15" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L16" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="17" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L17" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="18" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L18" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="19" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L19" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="20" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L20" t="s">
+        <v>211</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView topLeftCell="H1" workbookViewId="0">
@@ -1302,7 +1641,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G9"/>
   <sheetViews>
@@ -1437,7 +1776,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I7"/>
   <sheetViews>
@@ -1586,7 +1925,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H5"/>
   <sheetViews>
@@ -1717,7 +2056,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K7"/>
   <sheetViews>
@@ -1978,7 +2317,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L11"/>
   <sheetViews>
@@ -2150,7 +2489,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D1:F13"/>
   <sheetViews>
@@ -2316,7 +2655,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G13"/>
   <sheetViews>
@@ -3714,7 +4053,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="A20" sqref="A20:E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4157,6 +4496,146 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="38.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="37.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C1" t="s">
+        <v>225</v>
+      </c>
+      <c r="D1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="D2" t="s">
+        <v>146</v>
+      </c>
+      <c r="E2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="D3" t="s">
+        <v>147</v>
+      </c>
+      <c r="E3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="D4" t="s">
+        <v>148</v>
+      </c>
+      <c r="E4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="D5" t="s">
+        <v>149</v>
+      </c>
+      <c r="E5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="D6" t="s">
+        <v>150</v>
+      </c>
+      <c r="E6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="D7" t="s">
+        <v>151</v>
+      </c>
+      <c r="E7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -4167,7 +4646,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F83"/>
   <sheetViews>
@@ -4919,12 +5398,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4966,300 +5445,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L20"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5:L20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="39.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="22" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="255.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="B2" s="6">
-        <v>1</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="E2" s="6">
-        <v>0</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="I2" s="6">
-        <v>1</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5" t="str">
-        <f>"INSERT INTO ordrar(orderID, tjanstID, anstalldID, personID, betald, orderdatum, starttid, sluttid, aktiv, createdBy) VALUES('"&amp;A2&amp;"','"&amp;B2&amp;"','"&amp;C2&amp;"','"&amp;D2&amp;"','"&amp;E2&amp;"','"&amp;F2&amp;"','"&amp;G2&amp;"','"&amp;H2&amp;"','"&amp;I2&amp;"','"&amp;J2&amp;"')"</f>
-        <v>INSERT INTO ordrar(orderID, tjanstID, anstalldID, personID, betald, orderdatum, starttid, sluttid, aktiv, createdBy) VALUES('0F51A3C3-D37C-444D-9D9A-7DA5C995837C','1','A3B762F3-79F8-49B2-8722-354505C82FF4','9E0C52CD-9F2C-432C-A6C1-D2475B5315D3','0','2016-11-14 08:46:18.427','2016-11-15 08:36:14.330','2016-11-15 10:36:14.330','1','A3B762F3-79F8-49B2-8722-354505C82FF4')</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="L5" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="L6" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="L7" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="L8" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="L9" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="L10" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="L11" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="L12" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="L13" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="L14" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="L15" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="L16" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="17" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L17" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="18" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L18" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="19" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L19" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="20" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L20" t="s">
-        <v>211</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>